<commit_message>
finish project 1 pt 2
</commit_message>
<xml_diff>
--- a/src/task_2.2/vaputra_task2pt2.xlsx
+++ b/src/task_2.2/vaputra_task2pt2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>5.053311099832815</v>
+        <v>3.169575339336041</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>6.625558706462265</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -538,22 +538,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>3.169575339336041</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8.138741115249973</v>
+      </c>
+      <c r="D4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>5.053311099832815</v>
-      </c>
-      <c r="D4" t="n">
-        <v>8.837323747074519</v>
-      </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>6.625558706462265</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -567,13 +567,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>5.053311099832815</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>8.492653210238799</v>
+        <v>8.138741115249973</v>
       </c>
       <c r="D5" t="n">
-        <v>8.837323747074519</v>
+        <v>6.485151809645515</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -582,7 +582,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>6.625558706462265</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -596,22 +596,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>6.625558706462265</v>
+        <v>6.485151809645515</v>
       </c>
       <c r="C6" t="n">
-        <v>8.492653210238799</v>
+        <v>8.138741115249973</v>
       </c>
       <c r="D6" t="n">
-        <v>8.837323747074519</v>
+        <v>7.408513247150115</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>6.656502198941924</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -625,28 +625,28 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>6.656502198941924</v>
+        <v>7.408513247150115</v>
       </c>
       <c r="C7" t="n">
-        <v>8.492653210238799</v>
+        <v>8.138741115249973</v>
       </c>
       <c r="D7" t="n">
-        <v>8.837323747074519</v>
+        <v>14.73709075155531</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>7.656502198941924</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -654,28 +654,28 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>7.656502198941924</v>
+        <v>8.138741115249973</v>
       </c>
       <c r="C8" t="n">
-        <v>8.492653210238799</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D8" t="n">
-        <v>8.837323747074519</v>
+        <v>14.73709075155531</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" t="n">
-        <v>13.78801915806102</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -683,28 +683,28 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8.492653210238799</v>
+        <v>9.421325893840358</v>
       </c>
       <c r="C9" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D9" t="n">
-        <v>8.837323747074519</v>
+        <v>14.73709075155531</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>9.829272763663267</v>
+        <v>9.807491356914879</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>5.295365947822223</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -712,28 +712,28 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>8.837323747074519</v>
+        <v>9.807491356914879</v>
       </c>
       <c r="C10" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D10" t="n">
-        <v>9.921581891404649</v>
+        <v>14.73709075155531</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" t="n">
-        <v>9.829272763663267</v>
+        <v>15.41167070311852</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>5.295365947822223</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -741,28 +741,28 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>9.829272763663267</v>
+        <v>14.73709075155531</v>
       </c>
       <c r="C11" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D11" t="n">
-        <v>9.921581891404649</v>
+        <v>16.97318577314171</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G11" t="n">
-        <v>15.12463871148549</v>
+        <v>15.41167070311852</v>
       </c>
       <c r="H11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -770,22 +770,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>9.921581891404649</v>
+        <v>15.41167070311852</v>
       </c>
       <c r="C12" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D12" t="n">
-        <v>12.68553175162768</v>
+        <v>16.97318577314171</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G12" t="n">
-        <v>15.12463871148549</v>
+        <v>16.41167070311852</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
@@ -799,13 +799,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>12.68553175162768</v>
+        <v>16.41167070311852</v>
       </c>
       <c r="C13" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D13" t="n">
-        <v>19.55479204266773</v>
+        <v>16.97318577314171</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="G13" t="n">
-        <v>15.12463871148549</v>
+        <v>16.60391311292053</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
@@ -828,13 +828,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>15.12463871148549</v>
+        <v>16.60391311292053</v>
       </c>
       <c r="C14" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D14" t="n">
-        <v>19.55479204266773</v>
+        <v>16.97318577314171</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>15.79433987134802</v>
+        <v>17.47154784418869</v>
       </c>
       <c r="H14" t="n">
         <v>2</v>
@@ -857,22 +857,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>15.79433987134802</v>
+        <v>16.97318577314171</v>
       </c>
       <c r="C15" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D15" t="n">
-        <v>19.55479204266773</v>
+        <v>23.65284525247422</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>16.1536418023474</v>
+        <v>17.47154784418869</v>
       </c>
       <c r="H15" t="n">
         <v>2</v>
@@ -886,22 +886,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>16.1536418023474</v>
+        <v>17.47154784418869</v>
       </c>
       <c r="C16" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D16" t="n">
-        <v>19.55479204266773</v>
+        <v>23.65284525247422</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>17.60005789983667</v>
+        <v>22.90028721768</v>
       </c>
       <c r="H16" t="n">
         <v>2</v>
@@ -915,25 +915,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>17.60005789983667</v>
+        <v>22.90028721768</v>
       </c>
       <c r="C17" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D17" t="n">
-        <v>19.55479204266773</v>
+        <v>23.65284525247422</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>17.60005789983667</v>
+        <v>23.98078800919883</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -944,22 +944,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19.55479204266773</v>
+        <v>23.65284525247422</v>
       </c>
       <c r="C18" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D18" t="n">
-        <v>23.24345691775543</v>
+        <v>35.20638964411476</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>23.38572613428676</v>
+        <v>23.98078800919883</v>
       </c>
       <c r="H18" t="n">
         <v>2</v>
@@ -973,13 +973,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>23.24345691775543</v>
+        <v>23.98078800919883</v>
       </c>
       <c r="C19" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D19" t="n">
-        <v>26.43646744924921</v>
+        <v>35.20638964411476</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>23.38572613428676</v>
+        <v>32.74586260200236</v>
       </c>
       <c r="H19" t="n">
         <v>2</v>
@@ -1002,13 +1002,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>23.38572613428676</v>
+        <v>32.74586260200236</v>
       </c>
       <c r="C20" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D20" t="n">
-        <v>26.43646744924921</v>
+        <v>35.20638964411476</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>28.73484731530317</v>
+        <v>37.14623208037837</v>
       </c>
       <c r="H20" t="n">
         <v>2</v>
@@ -1031,13 +1031,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>26.43646744924921</v>
+        <v>35.20638964411476</v>
       </c>
       <c r="C21" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D21" t="n">
-        <v>29.86001340778365</v>
+        <v>37.42007695739594</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>28.73484731530317</v>
+        <v>37.14623208037837</v>
       </c>
       <c r="H21" t="n">
         <v>2</v>
@@ -1060,13 +1060,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>28.73484731530317</v>
+        <v>37.14623208037837</v>
       </c>
       <c r="C22" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D22" t="n">
-        <v>29.86001340778365</v>
+        <v>37.42007695739594</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>29.55776082109779</v>
+        <v>38.06034753009004</v>
       </c>
       <c r="H22" t="n">
         <v>2</v>
@@ -1089,25 +1089,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>29.55776082109779</v>
+        <v>37.42007695739594</v>
       </c>
       <c r="C23" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D23" t="n">
-        <v>29.86001340778365</v>
+        <v>44.58582169547706</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>29.55776082109779</v>
+        <v>38.06034753009004</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1118,13 +1118,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>29.86001340778365</v>
+        <v>38.06034753009004</v>
       </c>
       <c r="C24" t="n">
-        <v>39.08413190761105</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="D24" t="n">
-        <v>30.42421176224238</v>
+        <v>44.58582169547706</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>34.73220600556079</v>
+        <v>45.2069290191166</v>
       </c>
       <c r="H24" t="n">
         <v>2</v>
@@ -1147,13 +1147,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>30.42421176224238</v>
+        <v>39.59300617245973</v>
       </c>
       <c r="C25" t="n">
-        <v>39.08413190761105</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="D25" t="n">
-        <v>47.43713729935631</v>
+        <v>44.58582169547706</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1162,13 +1162,13 @@
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>34.73220600556079</v>
+        <v>39.68114315262481</v>
       </c>
       <c r="H25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>5.61392284665687</v>
       </c>
     </row>
     <row r="26">
@@ -1176,13 +1176,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>34.73220600556079</v>
+        <v>39.68114315262481</v>
       </c>
       <c r="C26" t="n">
-        <v>39.08413190761105</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="D26" t="n">
-        <v>47.43713729935631</v>
+        <v>44.58582169547706</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>39.43316658407596</v>
+        <v>45.29506599928168</v>
       </c>
       <c r="H26" t="n">
         <v>2</v>
@@ -1205,13 +1205,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>39.08413190761105</v>
+        <v>44.58582169547706</v>
       </c>
       <c r="C27" t="n">
-        <v>57.94983871499851</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="D27" t="n">
-        <v>47.43713729935631</v>
+        <v>48.28833700230273</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1220,13 +1220,13 @@
         <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>45.24548365601014</v>
+        <v>45.29506599928168</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" t="n">
-        <v>0.3490346764649033</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1234,13 +1234,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>45.24548365601014</v>
+        <v>45.29506599928168</v>
       </c>
       <c r="C28" t="n">
-        <v>57.94983871499851</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="D28" t="n">
-        <v>47.43713729935631</v>
+        <v>48.28833700230273</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -1249,7 +1249,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>45.59451833247505</v>
+        <v>46.21650728901144</v>
       </c>
       <c r="H28" t="n">
         <v>2</v>
@@ -1263,13 +1263,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>45.59451833247505</v>
+        <v>46.21650728901144</v>
       </c>
       <c r="C29" t="n">
-        <v>57.94983871499851</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="D29" t="n">
-        <v>47.43713729935631</v>
+        <v>48.28833700230273</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>45.59451833247505</v>
+        <v>46.21650728901144</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1292,13 +1292,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>47.43713729935631</v>
+        <v>48.28833700230273</v>
       </c>
       <c r="C30" t="n">
-        <v>57.94983871499851</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="D30" t="n">
-        <v>50.35250972009362</v>
+        <v>48.44608264064718</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -1307,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>50.20367340876582</v>
+        <v>51.30764144995734</v>
       </c>
       <c r="H30" t="n">
         <v>2</v>
@@ -1321,28 +1321,28 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>50.20367340876582</v>
+        <v>48.33008059472795</v>
       </c>
       <c r="C31" t="n">
-        <v>57.94983871499851</v>
+        <v>48.5944518813787</v>
       </c>
       <c r="D31" t="n">
-        <v>50.35250972009362</v>
+        <v>48.44608264064718</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>50.20367340876582</v>
+        <v>49.25459749124284</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>2.977560855229392</v>
       </c>
     </row>
     <row r="32">
@@ -1350,28 +1350,28 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>50.35250972009362</v>
+        <v>48.44608264064718</v>
       </c>
       <c r="C32" t="n">
-        <v>57.94983871499851</v>
+        <v>48.5944518813787</v>
       </c>
       <c r="D32" t="n">
-        <v>81.02472614256271</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>55.63930704918696</v>
+        <v>49.25459749124284</v>
       </c>
       <c r="H32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>2.977560855229392</v>
       </c>
     </row>
     <row r="33">
@@ -1379,28 +1379,28 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>55.63930704918696</v>
+        <v>48.5944518813787</v>
       </c>
       <c r="C33" t="n">
-        <v>57.94983871499851</v>
+        <v>49.10610093711528</v>
       </c>
       <c r="D33" t="n">
-        <v>81.02472614256271</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>55.63930704918696</v>
+        <v>49.25459749124284</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>2.977560855229392</v>
       </c>
     </row>
     <row r="34">
@@ -1408,28 +1408,28 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>57.94983871499851</v>
+        <v>49.10610093711528</v>
       </c>
       <c r="C34" t="n">
-        <v>64.38695999481514</v>
+        <v>54.59701439868512</v>
       </c>
       <c r="D34" t="n">
-        <v>81.02472614256271</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G34" t="n">
-        <v>63.88015706189928</v>
+        <v>49.25459749124284</v>
       </c>
       <c r="H34" t="n">
         <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>2.977560855229392</v>
       </c>
     </row>
     <row r="35">
@@ -1437,28 +1437,28 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>63.88015706189928</v>
+        <v>49.25459749124284</v>
       </c>
       <c r="C35" t="n">
-        <v>64.38695999481514</v>
+        <v>54.59701439868512</v>
       </c>
       <c r="D35" t="n">
-        <v>81.02472614256271</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35" t="n">
-        <v>63.88015706189928</v>
+        <v>51.72720452459036</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>2.977560855229392</v>
       </c>
     </row>
     <row r="36">
@@ -1466,28 +1466,28 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>64.38695999481514</v>
+        <v>51.72720452459036</v>
       </c>
       <c r="C36" t="n">
-        <v>65.39739671573399</v>
+        <v>54.59701439868512</v>
       </c>
       <c r="D36" t="n">
-        <v>81.02472614256271</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G36" t="n">
-        <v>65.12514999087695</v>
+        <v>53.90122493533674</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>2.977560855229392</v>
       </c>
     </row>
     <row r="37">
@@ -1495,25 +1495,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>65.12514999087695</v>
+        <v>53.90122493533674</v>
       </c>
       <c r="C37" t="n">
-        <v>65.39739671573399</v>
+        <v>54.59701439868512</v>
       </c>
       <c r="D37" t="n">
-        <v>81.02472614256271</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>65.12514999087695</v>
+        <v>56.87878579056613</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -1524,25 +1524,25 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>65.39739671573399</v>
+        <v>54.16272454472395</v>
       </c>
       <c r="C38" t="n">
-        <v>78.57794270834573</v>
+        <v>54.59701439868512</v>
       </c>
       <c r="D38" t="n">
-        <v>81.02472614256271</v>
+        <v>55.58719103370387</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38" t="n">
-        <v>69.80866245375972</v>
+        <v>56.87878579056613</v>
       </c>
       <c r="H38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -1553,28 +1553,28 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>69.80866245375972</v>
+        <v>54.59701439868512</v>
       </c>
       <c r="C39" t="n">
-        <v>78.57794270834573</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D39" t="n">
-        <v>81.02472614256271</v>
+        <v>55.58719103370387</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G39" t="n">
-        <v>69.80866245375972</v>
+        <v>54.72011092105741</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>2.281771391881009</v>
       </c>
     </row>
     <row r="40">
@@ -1582,25 +1582,25 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>78.57794270834573</v>
+        <v>54.72011092105741</v>
       </c>
       <c r="C40" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D40" t="n">
-        <v>81.02472614256271</v>
+        <v>55.58719103370387</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G40" t="n">
-        <v>79.67732077626485</v>
+        <v>57.00188231293842</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -1611,25 +1611,25 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>79.67732077626485</v>
+        <v>55.58719103370387</v>
       </c>
       <c r="C41" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D41" t="n">
-        <v>81.02472614256271</v>
+        <v>60.1724551261176</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G41" t="n">
-        <v>79.67732077626485</v>
+        <v>57.00188231293842</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -1640,22 +1640,22 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>81.02472614256271</v>
+        <v>57.00188231293842</v>
       </c>
       <c r="C42" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D42" t="n">
-        <v>83.20026646979653</v>
+        <v>60.1724551261176</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
-        <v>81.93475412986159</v>
+        <v>65.21578129526294</v>
       </c>
       <c r="H42" t="n">
         <v>2</v>
@@ -1669,25 +1669,25 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>81.93475412986159</v>
+        <v>60.1724551261176</v>
       </c>
       <c r="C43" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D43" t="n">
-        <v>83.20026646979653</v>
+        <v>60.59226235745296</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G43" t="n">
-        <v>81.93475412986159</v>
+        <v>65.21578129526294</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -1698,22 +1698,22 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>83.20026646979653</v>
+        <v>60.59226235745296</v>
       </c>
       <c r="C44" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D44" t="n">
-        <v>83.79623874469762</v>
+        <v>61.32326452622092</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G44" t="n">
-        <v>89.4575546683181</v>
+        <v>65.21578129526294</v>
       </c>
       <c r="H44" t="n">
         <v>2</v>
@@ -1727,22 +1727,22 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>83.79623874469762</v>
+        <v>61.32326452622092</v>
       </c>
       <c r="C45" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D45" t="n">
-        <v>86.04151598562326</v>
+        <v>62.08108581709376</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G45" t="n">
-        <v>89.4575546683181</v>
+        <v>65.21578129526294</v>
       </c>
       <c r="H45" t="n">
         <v>2</v>
@@ -1756,22 +1756,22 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>86.04151598562326</v>
+        <v>62.08108581709376</v>
       </c>
       <c r="C46" t="n">
-        <v>91.48337238855505</v>
+        <v>62.710505907475</v>
       </c>
       <c r="D46" t="n">
-        <v>86.72793152326601</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G46" t="n">
-        <v>89.4575546683181</v>
+        <v>65.21578129526294</v>
       </c>
       <c r="H46" t="n">
         <v>2</v>
@@ -1785,28 +1785,28 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>86.72793152326601</v>
+        <v>62.710505907475</v>
       </c>
       <c r="C47" t="n">
-        <v>91.48337238855505</v>
+        <v>65.13722836164624</v>
       </c>
       <c r="D47" t="n">
-        <v>87.03464422565852</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G47" t="n">
-        <v>89.4575546683181</v>
+        <v>63.90712644758617</v>
       </c>
       <c r="H47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>2.505275387787947</v>
       </c>
     </row>
     <row r="48">
@@ -1814,22 +1814,22 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>87.03464422565852</v>
+        <v>63.90712644758617</v>
       </c>
       <c r="C48" t="n">
-        <v>91.48337238855505</v>
+        <v>65.13722836164624</v>
       </c>
       <c r="D48" t="n">
-        <v>96.45006574267454</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G48" t="n">
-        <v>89.4575546683181</v>
+        <v>66.41240183537411</v>
       </c>
       <c r="H48" t="n">
         <v>2</v>
@@ -1843,28 +1843,28 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>89.4575546683181</v>
+        <v>65.13722836164624</v>
       </c>
       <c r="C49" t="n">
-        <v>91.48337238855505</v>
+        <v>69.63037869372981</v>
       </c>
       <c r="D49" t="n">
-        <v>96.45006574267454</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G49" t="n">
-        <v>90.53714610367729</v>
+        <v>65.18210844277107</v>
       </c>
       <c r="H49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1.275173473727875</v>
       </c>
     </row>
     <row r="50">
@@ -1872,22 +1872,22 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>90.53714610367729</v>
+        <v>65.18210844277107</v>
       </c>
       <c r="C50" t="n">
-        <v>91.48337238855505</v>
+        <v>69.63037869372981</v>
       </c>
       <c r="D50" t="n">
-        <v>96.45006574267454</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G50" t="n">
-        <v>94.21670024943495</v>
+        <v>66.45728191649894</v>
       </c>
       <c r="H50" t="n">
         <v>2</v>
@@ -1901,28 +1901,28 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>91.48337238855505</v>
+        <v>66.45728191649894</v>
       </c>
       <c r="C51" t="n">
-        <v>98.29298842446259</v>
+        <v>69.63037869372981</v>
       </c>
       <c r="D51" t="n">
-        <v>96.45006574267454</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G51" t="n">
-        <v>91.94093393330397</v>
+        <v>69.71310295798027</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51" t="n">
-        <v>2.733327860879896</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1930,22 +1930,22 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>91.94093393330397</v>
+        <v>67.06406420534587</v>
       </c>
       <c r="C52" t="n">
-        <v>98.29298842446259</v>
+        <v>69.63037869372981</v>
       </c>
       <c r="D52" t="n">
-        <v>96.45006574267454</v>
+        <v>67.70549884895826</v>
       </c>
       <c r="E52" t="n">
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G52" t="n">
-        <v>94.67426179418386</v>
+        <v>69.71310295798027</v>
       </c>
       <c r="H52" t="n">
         <v>2</v>
@@ -1959,22 +1959,22 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>94.67426179418386</v>
+        <v>67.70549884895826</v>
       </c>
       <c r="C53" t="n">
-        <v>98.29298842446259</v>
+        <v>69.63037869372981</v>
       </c>
       <c r="D53" t="n">
-        <v>96.45006574267454</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G53" t="n">
-        <v>99.37358796113557</v>
+        <v>69.71310295798027</v>
       </c>
       <c r="H53" t="n">
         <v>2</v>
@@ -1988,28 +1988,28 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>96.45006574267454</v>
+        <v>69.63037869372981</v>
       </c>
       <c r="C54" t="n">
-        <v>98.29298842446259</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D54" t="n">
-        <v>107.3493888410137</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G54" t="n">
-        <v>99.37358796113557</v>
+        <v>69.72513190805842</v>
       </c>
       <c r="H54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>0.08272426425045865</v>
       </c>
     </row>
     <row r="55">
@@ -2017,28 +2017,28 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>98.29298842446259</v>
+        <v>69.72513190805842</v>
       </c>
       <c r="C55" t="n">
-        <v>101.793201300613</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D55" t="n">
-        <v>107.3493888410137</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G55" t="n">
-        <v>100.321422847964</v>
+        <v>69.80785617230887</v>
       </c>
       <c r="H55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I55" t="n">
-        <v>1.080599536672977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2046,22 +2046,22 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>100.321422847964</v>
+        <v>69.80785617230887</v>
       </c>
       <c r="C56" t="n">
-        <v>101.793201300613</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D56" t="n">
-        <v>107.3493888410137</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G56" t="n">
-        <v>101.402022384637</v>
+        <v>70.04965493915753</v>
       </c>
       <c r="H56" t="n">
         <v>2</v>
@@ -2075,22 +2075,22 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>101.402022384637</v>
+        <v>70.04965493915753</v>
       </c>
       <c r="C57" t="n">
-        <v>101.793201300613</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D57" t="n">
-        <v>107.3493888410137</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G57" t="n">
-        <v>101.83519716273</v>
+        <v>70.69629850918575</v>
       </c>
       <c r="H57" t="n">
         <v>2</v>
@@ -2104,28 +2104,28 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>101.793201300613</v>
+        <v>70.69629850918575</v>
       </c>
       <c r="C58" t="n">
-        <v>110.407058846389</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D58" t="n">
-        <v>107.3493888410137</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G58" t="n">
-        <v>102.6629648579485</v>
+        <v>75.83147610853624</v>
       </c>
       <c r="H58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I58" t="n">
-        <v>0.0419958621169485</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2133,22 +2133,22 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>102.6629648579485</v>
+        <v>72.8278191003489</v>
       </c>
       <c r="C59" t="n">
-        <v>110.407058846389</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D59" t="n">
-        <v>107.3493888410137</v>
+        <v>81.81254886290155</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G59" t="n">
-        <v>102.7049607200655</v>
+        <v>75.83147610853624</v>
       </c>
       <c r="H59" t="n">
         <v>2</v>
@@ -2162,22 +2162,22 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>102.7049607200655</v>
+        <v>75.83147610853624</v>
       </c>
       <c r="C60" t="n">
-        <v>110.407058846389</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D60" t="n">
-        <v>107.3493888410137</v>
+        <v>81.81254886290155</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G60" t="n">
-        <v>104.1626969774185</v>
+        <v>76.21993394351146</v>
       </c>
       <c r="H60" t="n">
         <v>2</v>
@@ -2191,25 +2191,25 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>104.1626969774185</v>
+        <v>76.21993394351146</v>
       </c>
       <c r="C61" t="n">
-        <v>110.407058846389</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D61" t="n">
-        <v>107.3493888410137</v>
+        <v>81.81254886290155</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G61" t="n">
-        <v>104.1626969774185</v>
+        <v>90.80243138963318</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -2220,22 +2220,22 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>107.3493888410137</v>
+        <v>81.81254886290155</v>
       </c>
       <c r="C62" t="n">
-        <v>110.407058846389</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D62" t="n">
-        <v>107.6168650534381</v>
+        <v>82.02237483894737</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G62" t="n">
-        <v>111.5733606309927</v>
+        <v>90.80243138963318</v>
       </c>
       <c r="H62" t="n">
         <v>2</v>
@@ -2249,22 +2249,22 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>107.6168650534381</v>
+        <v>82.02237483894737</v>
       </c>
       <c r="C63" t="n">
-        <v>110.407058846389</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="D63" t="n">
-        <v>108.7907684696321</v>
+        <v>86.93693727227912</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G63" t="n">
-        <v>111.5733606309927</v>
+        <v>90.80243138963318</v>
       </c>
       <c r="H63" t="n">
         <v>2</v>
@@ -2278,28 +2278,28 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>108.7907684696321</v>
+        <v>83.19239404881316</v>
       </c>
       <c r="C64" t="n">
-        <v>110.407058846389</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D64" t="n">
-        <v>110.7611784540195</v>
+        <v>86.93693727227912</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G64" t="n">
-        <v>111.5733606309927</v>
+        <v>84.50966439592405</v>
       </c>
       <c r="H64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>7.610037340820028</v>
       </c>
     </row>
     <row r="65">
@@ -2307,28 +2307,28 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>110.407058846389</v>
+        <v>84.50966439592405</v>
       </c>
       <c r="C65" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D65" t="n">
-        <v>110.7611784540195</v>
+        <v>86.93693727227912</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G65" t="n">
-        <v>111.1766245791976</v>
+        <v>92.11970173674408</v>
       </c>
       <c r="H65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I65" t="n">
-        <v>1.166301784603732</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2336,28 +2336,28 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>110.7611784540195</v>
+        <v>86.93693727227912</v>
       </c>
       <c r="C66" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D66" t="n">
-        <v>114.5348805208857</v>
+        <v>92.88422193229009</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G66" t="n">
-        <v>111.1766245791976</v>
+        <v>92.11970173674408</v>
       </c>
       <c r="H66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I66" t="n">
-        <v>1.166301784603732</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2365,22 +2365,22 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>111.1766245791976</v>
+        <v>92.11970173674408</v>
       </c>
       <c r="C67" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D67" t="n">
-        <v>114.5348805208857</v>
+        <v>92.88422193229009</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G67" t="n">
-        <v>112.3429263638013</v>
+        <v>92.96658636858891</v>
       </c>
       <c r="H67" t="n">
         <v>2</v>
@@ -2394,22 +2394,22 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>112.3429263638013</v>
+        <v>92.88422193229009</v>
       </c>
       <c r="C68" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D68" t="n">
-        <v>114.5348805208857</v>
+        <v>99.2922249695123</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G68" t="n">
-        <v>114.1803288267654</v>
+        <v>92.96658636858891</v>
       </c>
       <c r="H68" t="n">
         <v>2</v>
@@ -2423,22 +2423,22 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>114.1803288267654</v>
+        <v>92.96658636858891</v>
       </c>
       <c r="C69" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D69" t="n">
-        <v>114.5348805208857</v>
+        <v>99.2922249695123</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G69" t="n">
-        <v>114.6151557831389</v>
+        <v>96.74756013802684</v>
       </c>
       <c r="H69" t="n">
         <v>2</v>
@@ -2452,22 +2452,22 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>114.5348805208857</v>
+        <v>96.74756013802684</v>
       </c>
       <c r="C70" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D70" t="n">
-        <v>123.6700042264678</v>
+        <v>99.2922249695123</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G70" t="n">
-        <v>114.6151557831389</v>
+        <v>97.25253925839192</v>
       </c>
       <c r="H70" t="n">
         <v>2</v>
@@ -2481,22 +2481,22 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>114.6151557831389</v>
+        <v>97.25253925839192</v>
       </c>
       <c r="C71" t="n">
-        <v>114.6238765511951</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D71" t="n">
-        <v>123.6700042264678</v>
+        <v>99.2922249695123</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G71" t="n">
-        <v>117.0671923114816</v>
+        <v>100.3832661536643</v>
       </c>
       <c r="H71" t="n">
         <v>2</v>
@@ -2510,28 +2510,28 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>114.6238765511951</v>
+        <v>99.2922249695123</v>
       </c>
       <c r="C72" t="n">
-        <v>120.006009458909</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D72" t="n">
-        <v>123.6700042264678</v>
+        <v>104.7356607495179</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G72" t="n">
-        <v>116.4108737355454</v>
+        <v>100.3832661536643</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I72" t="n">
-        <v>2.443315760286481</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2539,22 +2539,22 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>116.4108737355454</v>
+        <v>100.3832661536643</v>
       </c>
       <c r="C73" t="n">
-        <v>120.006009458909</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="D73" t="n">
-        <v>123.6700042264678</v>
+        <v>104.7356607495179</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G73" t="n">
-        <v>118.8541894958319</v>
+        <v>108.2791433823418</v>
       </c>
       <c r="H73" t="n">
         <v>2</v>
@@ -2568,28 +2568,28 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>118.8541894958319</v>
+        <v>104.6702829739266</v>
       </c>
       <c r="C74" t="n">
-        <v>120.006009458909</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D74" t="n">
-        <v>123.6700042264678</v>
+        <v>104.7356607495179</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G74" t="n">
-        <v>123.6233085556322</v>
+        <v>105.4102054046698</v>
       </c>
       <c r="H74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>3.608860408415254</v>
       </c>
     </row>
     <row r="75">
@@ -2597,28 +2597,28 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>120.006009458909</v>
+        <v>104.7356607495179</v>
       </c>
       <c r="C75" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D75" t="n">
-        <v>123.6700042264678</v>
+        <v>116.960096822894</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G75" t="n">
-        <v>120.1984250127382</v>
+        <v>105.4102054046698</v>
       </c>
       <c r="H75" t="n">
         <v>1</v>
       </c>
       <c r="I75" t="n">
-        <v>3.617299096723215</v>
+        <v>3.608860408415254</v>
       </c>
     </row>
     <row r="76">
@@ -2626,22 +2626,22 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>120.1984250127382</v>
+        <v>105.4102054046698</v>
       </c>
       <c r="C76" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D76" t="n">
-        <v>123.6700042264678</v>
+        <v>116.960096822894</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G76" t="n">
-        <v>123.8157241094614</v>
+        <v>109.019065813085</v>
       </c>
       <c r="H76" t="n">
         <v>2</v>
@@ -2655,22 +2655,22 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>123.6700042264678</v>
+        <v>109.019065813085</v>
       </c>
       <c r="C77" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D77" t="n">
-        <v>123.9093186998149</v>
+        <v>116.960096822894</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G77" t="n">
-        <v>123.8157241094614</v>
+        <v>111.8041096295354</v>
       </c>
       <c r="H77" t="n">
         <v>2</v>
@@ -2684,22 +2684,22 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>123.8157241094614</v>
+        <v>111.8041096295354</v>
       </c>
       <c r="C78" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D78" t="n">
-        <v>123.9093186998149</v>
+        <v>116.960096822894</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G78" t="n">
-        <v>127.3449532221807</v>
+        <v>116.2252209351316</v>
       </c>
       <c r="H78" t="n">
         <v>2</v>
@@ -2713,13 +2713,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>123.9093186998149</v>
+        <v>116.2252209351316</v>
       </c>
       <c r="C79" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D79" t="n">
-        <v>125.6812226649885</v>
+        <v>116.960096822894</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="G79" t="n">
-        <v>127.3449532221807</v>
+        <v>120.4874678694877</v>
       </c>
       <c r="H79" t="n">
         <v>2</v>
@@ -2742,13 +2742,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>125.6812226649885</v>
+        <v>116.960096822894</v>
       </c>
       <c r="C80" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D80" t="n">
-        <v>127.1446978082817</v>
+        <v>121.0807006507304</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -2757,7 +2757,7 @@
         <v>2</v>
       </c>
       <c r="G80" t="n">
-        <v>127.3449532221807</v>
+        <v>120.4874678694877</v>
       </c>
       <c r="H80" t="n">
         <v>2</v>
@@ -2771,22 +2771,22 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>127.1446978082817</v>
+        <v>120.4874678694877</v>
       </c>
       <c r="C81" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D81" t="n">
-        <v>141.3862966004368</v>
+        <v>121.0807006507304</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G81" t="n">
-        <v>127.3449532221807</v>
+        <v>122.724358298895</v>
       </c>
       <c r="H81" t="n">
         <v>2</v>
@@ -2800,13 +2800,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>127.3449532221807</v>
+        <v>121.0807006507304</v>
       </c>
       <c r="C82" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D82" t="n">
-        <v>141.3862966004368</v>
+        <v>123.5025277420555</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -2815,7 +2815,7 @@
         <v>2</v>
       </c>
       <c r="G82" t="n">
-        <v>132.8286251895885</v>
+        <v>122.724358298895</v>
       </c>
       <c r="H82" t="n">
         <v>2</v>
@@ -2829,13 +2829,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>132.8286251895885</v>
+        <v>122.724358298895</v>
       </c>
       <c r="C83" t="n">
-        <v>133.0377263757472</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D83" t="n">
-        <v>141.3862966004368</v>
+        <v>123.5025277420555</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
       <c r="G83" t="n">
-        <v>133.9477557078904</v>
+        <v>124.6326470248789</v>
       </c>
       <c r="H83" t="n">
         <v>2</v>
@@ -2858,13 +2858,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>133.0377263757472</v>
+        <v>123.5025277420555</v>
       </c>
       <c r="C84" t="n">
-        <v>144.1831353853669</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D84" t="n">
-        <v>141.3862966004368</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -2873,13 +2873,13 @@
         <v>2</v>
       </c>
       <c r="G84" t="n">
-        <v>133.7418379536107</v>
+        <v>124.6326470248789</v>
       </c>
       <c r="H84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I84" t="n">
-        <v>0.910029332143182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2887,13 +2887,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>133.7418379536107</v>
+        <v>124.6326470248789</v>
       </c>
       <c r="C85" t="n">
-        <v>144.1831353853669</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D85" t="n">
-        <v>141.3862966004368</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
@@ -2902,7 +2902,7 @@
         <v>1</v>
       </c>
       <c r="G85" t="n">
-        <v>134.6518672857539</v>
+        <v>131.586301143804</v>
       </c>
       <c r="H85" t="n">
         <v>2</v>
@@ -2916,13 +2916,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>134.6518672857539</v>
+        <v>131.586301143804</v>
       </c>
       <c r="C86" t="n">
-        <v>144.1831353853669</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D86" t="n">
-        <v>141.3862966004368</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -2931,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>136.1773601168464</v>
+        <v>132.1868596338066</v>
       </c>
       <c r="H86" t="n">
         <v>2</v>
@@ -2945,13 +2945,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>136.1773601168464</v>
+        <v>132.1868596338066</v>
       </c>
       <c r="C87" t="n">
-        <v>144.1831353853669</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="D87" t="n">
-        <v>141.3862966004368</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
@@ -2960,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>136.1773601168464</v>
+        <v>132.1868596338066</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -2974,13 +2974,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>141.3862966004368</v>
+        <v>143.9518974519905</v>
       </c>
       <c r="C88" t="n">
-        <v>144.1831353853669</v>
+        <v>150.6332968939227</v>
       </c>
       <c r="D88" t="n">
-        <v>159.8603044057208</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -2989,10 +2989,10 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>146.1063032084575</v>
+        <v>144.1123926563245</v>
       </c>
       <c r="H88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I88" t="n">
         <v>0</v>
@@ -3003,28 +3003,28 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>144.1831353853669</v>
+        <v>144.1123926563245</v>
       </c>
       <c r="C89" t="n">
-        <v>147.3993615556883</v>
+        <v>150.6332968939227</v>
       </c>
       <c r="D89" t="n">
-        <v>159.8603044057208</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>146.1649989769789</v>
+        <v>144.1123926563245</v>
       </c>
       <c r="H89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="n">
-        <v>1.92316782309058</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3032,13 +3032,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>146.1649989769789</v>
+        <v>147.7280753136199</v>
       </c>
       <c r="C90" t="n">
-        <v>147.3993615556883</v>
+        <v>150.6332968939227</v>
       </c>
       <c r="D90" t="n">
-        <v>159.8603044057208</v>
+        <v>148.6118815431635</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -3047,7 +3047,7 @@
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>148.0881668000695</v>
+        <v>154.6996718470792</v>
       </c>
       <c r="H90" t="n">
         <v>2</v>
@@ -3061,13 +3061,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>147.3993615556883</v>
+        <v>148.6118815431635</v>
       </c>
       <c r="C91" t="n">
-        <v>171.1003516527272</v>
+        <v>150.6332968939227</v>
       </c>
       <c r="D91" t="n">
-        <v>159.8603044057208</v>
+        <v>157.3552005686082</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
@@ -3076,13 +3076,13 @@
         <v>1</v>
       </c>
       <c r="G91" t="n">
-        <v>147.8707268109758</v>
+        <v>154.6996718470792</v>
       </c>
       <c r="H91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I91" t="n">
-        <v>0.6888052443812001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -3090,28 +3090,28 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>147.8707268109758</v>
+        <v>150.6332968939227</v>
       </c>
       <c r="C92" t="n">
-        <v>171.1003516527272</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D92" t="n">
-        <v>159.8603044057208</v>
+        <v>157.3552005686082</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G92" t="n">
-        <v>148.559532055357</v>
+        <v>150.822057873592</v>
       </c>
       <c r="H92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I92" t="n">
-        <v>0</v>
+        <v>4.066374953156497</v>
       </c>
     </row>
     <row r="93">
@@ -3119,25 +3119,25 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>148.559532055357</v>
+        <v>150.822057873592</v>
       </c>
       <c r="C93" t="n">
-        <v>171.1003516527272</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D93" t="n">
-        <v>159.8603044057208</v>
+        <v>157.3552005686082</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93" t="n">
-        <v>148.559532055357</v>
+        <v>154.8884328267485</v>
       </c>
       <c r="H93" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I93" t="n">
         <v>0</v>
@@ -3148,13 +3148,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>159.8603044057208</v>
+        <v>154.8884328267485</v>
       </c>
       <c r="C94" t="n">
-        <v>171.1003516527272</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D94" t="n">
-        <v>172.2097522579122</v>
+        <v>157.3552005686082</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>160.0096892051783</v>
+        <v>155.8030590750718</v>
       </c>
       <c r="H94" t="n">
         <v>2</v>
@@ -3177,13 +3177,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>160.0096892051783</v>
+        <v>155.8030590750718</v>
       </c>
       <c r="C95" t="n">
-        <v>171.1003516527272</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D95" t="n">
-        <v>172.2097522579122</v>
+        <v>157.3552005686082</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>160.0096892051783</v>
+        <v>155.8030590750718</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
@@ -3206,13 +3206,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>171.1003516527272</v>
+        <v>157.3552005686082</v>
       </c>
       <c r="C96" t="n">
-        <v>174.3078909872066</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D96" t="n">
-        <v>172.2097522579122</v>
+        <v>159.0160334401216</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -3221,10 +3221,10 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>172.5768901584282</v>
+        <v>162.0616511318598</v>
       </c>
       <c r="H96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I96" t="n">
         <v>0</v>
@@ -3235,13 +3235,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>172.2097522579122</v>
+        <v>159.0160334401216</v>
       </c>
       <c r="C97" t="n">
-        <v>174.3078909872066</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D97" t="n">
-        <v>177.2517621425689</v>
+        <v>164.3387388408639</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -3250,10 +3250,10 @@
         <v>1</v>
       </c>
       <c r="G97" t="n">
-        <v>172.5768901584282</v>
+        <v>162.0616511318598</v>
       </c>
       <c r="H97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I97" t="n">
         <v>0</v>
@@ -3264,13 +3264,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>172.5768901584282</v>
+        <v>162.0616511318598</v>
       </c>
       <c r="C98" t="n">
-        <v>174.3078909872066</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D98" t="n">
-        <v>177.2517621425689</v>
+        <v>164.3387388408639</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -3279,7 +3279,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>173.7191795600814</v>
+        <v>169.0396054422304</v>
       </c>
       <c r="H98" t="n">
         <v>2</v>
@@ -3293,25 +3293,25 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>173.7191795600814</v>
+        <v>164.3387388408639</v>
       </c>
       <c r="C99" t="n">
-        <v>174.3078909872066</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D99" t="n">
-        <v>177.2517621425689</v>
+        <v>174.4734415978043</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" t="n">
-        <v>173.7191795600814</v>
+        <v>169.0396054422304</v>
       </c>
       <c r="H99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I99" t="n">
         <v>0</v>
@@ -3322,13 +3322,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>174.3078909872066</v>
+        <v>169.0396054422304</v>
       </c>
       <c r="C100" t="n">
-        <v>176.3243131049305</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D100" t="n">
-        <v>177.2517621425689</v>
+        <v>174.4734415978043</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -3337,10 +3337,10 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>176.8811939281362</v>
+        <v>172.6549550681713</v>
       </c>
       <c r="H100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100" t="n">
         <v>0</v>
@@ -3351,25 +3351,25 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>176.3243131049305</v>
+        <v>172.6549550681713</v>
       </c>
       <c r="C101" t="n">
-        <v>181.1728690220336</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D101" t="n">
-        <v>177.2517621425689</v>
+        <v>174.4734415978043</v>
       </c>
       <c r="E101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>176.8811939281362</v>
+        <v>172.6549550681713</v>
       </c>
       <c r="H101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="n">
         <v>0</v>
@@ -3380,13 +3380,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>176.8811939281362</v>
+        <v>174.4734415978043</v>
       </c>
       <c r="C102" t="n">
-        <v>181.1728690220336</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D102" t="n">
-        <v>177.2517621425689</v>
+        <v>177.4221761837777</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
@@ -3395,10 +3395,10 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>179.9833304041622</v>
+        <v>179.3139176245687</v>
       </c>
       <c r="H102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I102" t="n">
         <v>0</v>
@@ -3409,13 +3409,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>177.2517621425689</v>
+        <v>177.4221761837777</v>
       </c>
       <c r="C103" t="n">
-        <v>181.1728690220336</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D103" t="n">
-        <v>178.3558829046114</v>
+        <v>177.7405147810179</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
@@ -3424,10 +3424,10 @@
         <v>1</v>
       </c>
       <c r="G103" t="n">
-        <v>179.9833304041622</v>
+        <v>179.3139176245687</v>
       </c>
       <c r="H103" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I103" t="n">
         <v>0</v>
@@ -3438,13 +3438,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>178.3558829046114</v>
+        <v>177.7405147810179</v>
       </c>
       <c r="C104" t="n">
-        <v>181.1728690220336</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D104" t="n">
-        <v>194.280381107672</v>
+        <v>186.6262147831773</v>
       </c>
       <c r="E104" t="n">
         <v>0</v>
@@ -3453,10 +3453,10 @@
         <v>2</v>
       </c>
       <c r="G104" t="n">
-        <v>179.9833304041622</v>
+        <v>179.3139176245687</v>
       </c>
       <c r="H104" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I104" t="n">
         <v>0</v>
@@ -3467,13 +3467,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>179.9833304041622</v>
+        <v>179.3139176245687</v>
       </c>
       <c r="C105" t="n">
-        <v>181.1728690220336</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D105" t="n">
-        <v>194.280381107672</v>
+        <v>186.6262147831773</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -3482,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="G105" t="n">
-        <v>181.4362731741803</v>
+        <v>181.632196955772</v>
       </c>
       <c r="H105" t="n">
         <v>2</v>
@@ -3496,28 +3496,28 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>181.1728690220336</v>
+        <v>181.632196955772</v>
       </c>
       <c r="C106" t="n">
-        <v>184.9874551208605</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D106" t="n">
-        <v>194.280381107672</v>
+        <v>186.6262147831773</v>
       </c>
       <c r="E106" t="n">
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>183.2426167598937</v>
+        <v>182.8758158527237</v>
       </c>
       <c r="H106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I106" t="n">
-        <v>0.263404152146677</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -3525,25 +3525,25 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>183.2426167598937</v>
+        <v>182.8758158527237</v>
       </c>
       <c r="C107" t="n">
-        <v>184.9874551208605</v>
+        <v>185.399770066837</v>
       </c>
       <c r="D107" t="n">
-        <v>194.280381107672</v>
+        <v>186.6262147831773</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G107" t="n">
-        <v>183.5060209120403</v>
+        <v>182.8758158527237</v>
       </c>
       <c r="H107" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I107" t="n">
         <v>0</v>
@@ -3554,13 +3554,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>183.5060209120403</v>
+        <v>185.399770066837</v>
       </c>
       <c r="C108" t="n">
-        <v>184.9874551208605</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D108" t="n">
-        <v>194.280381107672</v>
+        <v>186.6262147831773</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -3569,10 +3569,10 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
-        <v>185.1725711817084</v>
+        <v>186.6915573362796</v>
       </c>
       <c r="H108" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I108" t="n">
         <v>0</v>
@@ -3583,13 +3583,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>184.9874551208605</v>
+        <v>186.6262147831773</v>
       </c>
       <c r="C109" t="n">
-        <v>199.7028686340113</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D109" t="n">
-        <v>194.280381107672</v>
+        <v>190.3184760060806</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="G109" t="n">
-        <v>189.1812414930419</v>
+        <v>186.6915573362796</v>
       </c>
       <c r="H109" t="n">
         <v>1</v>
       </c>
       <c r="I109" t="n">
-        <v>0.1851160608478892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -3612,13 +3612,13 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>189.1812414930419</v>
+        <v>186.6915573362796</v>
       </c>
       <c r="C110" t="n">
-        <v>199.7028686340113</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D110" t="n">
-        <v>194.280381107672</v>
+        <v>190.3184760060806</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -3627,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="G110" t="n">
-        <v>189.3663575538898</v>
+        <v>188.4362119291893</v>
       </c>
       <c r="H110" t="n">
         <v>2</v>
@@ -3641,13 +3641,13 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>189.3663575538898</v>
+        <v>188.4362119291893</v>
       </c>
       <c r="C111" t="n">
-        <v>199.7028686340113</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D111" t="n">
-        <v>194.280381107672</v>
+        <v>190.3184760060806</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
@@ -3656,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>189.3663575538898</v>
+        <v>188.4362119291893</v>
       </c>
       <c r="H111" t="n">
         <v>0</v>
@@ -3670,13 +3670,13 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>194.280381107672</v>
+        <v>190.3184760060806</v>
       </c>
       <c r="C112" t="n">
-        <v>199.7028686340113</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D112" t="n">
-        <v>213.9558428915788</v>
+        <v>191.3789067149978</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="G112" t="n">
-        <v>198.4868784326875</v>
+        <v>192.2838046127802</v>
       </c>
       <c r="H112" t="n">
         <v>2</v>
@@ -3699,25 +3699,25 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>198.4868784326875</v>
+        <v>191.3789067149978</v>
       </c>
       <c r="C113" t="n">
-        <v>199.7028686340113</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D113" t="n">
-        <v>213.9558428915788</v>
+        <v>192.905793596775</v>
       </c>
       <c r="E113" t="n">
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" t="n">
-        <v>198.4868784326875</v>
+        <v>192.2838046127802</v>
       </c>
       <c r="H113" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113" t="n">
         <v>0</v>
@@ -3728,13 +3728,13 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>199.7028686340113</v>
+        <v>192.2838046127802</v>
       </c>
       <c r="C114" t="n">
-        <v>206.2572859742533</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D114" t="n">
-        <v>213.9558428915788</v>
+        <v>192.905793596775</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
@@ -3743,10 +3743,10 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>199.7953513673442</v>
+        <v>192.8180466640652</v>
       </c>
       <c r="H114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I114" t="n">
         <v>0</v>
@@ -3757,13 +3757,13 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>199.7953513673442</v>
+        <v>192.8180466640652</v>
       </c>
       <c r="C115" t="n">
-        <v>206.2572859742533</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D115" t="n">
-        <v>213.9558428915788</v>
+        <v>192.905793596775</v>
       </c>
       <c r="E115" t="n">
         <v>0</v>
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="G115" t="n">
-        <v>199.7953513673442</v>
+        <v>192.8180466640652</v>
       </c>
       <c r="H115" t="n">
         <v>0</v>
@@ -3786,13 +3786,13 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>206.2572859742533</v>
+        <v>192.905793596775</v>
       </c>
       <c r="C116" t="n">
-        <v>209.7241258958845</v>
+        <v>243.8251434270446</v>
       </c>
       <c r="D116" t="n">
-        <v>213.9558428915788</v>
+        <v>200.8184214789345</v>
       </c>
       <c r="E116" t="n">
         <v>0</v>
@@ -3801,12 +3801,70 @@
         <v>0</v>
       </c>
       <c r="G116" t="n">
-        <v>209.1633629733049</v>
+        <v>212.1150871372558</v>
       </c>
       <c r="H116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>200.8184214789345</v>
+      </c>
+      <c r="C117" t="n">
+        <v>243.8251434270446</v>
+      </c>
+      <c r="D117" t="n">
+        <v>204.9710859665115</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1</v>
+      </c>
+      <c r="G117" t="n">
+        <v>212.1150871372558</v>
+      </c>
+      <c r="H117" t="n">
+        <v>2</v>
+      </c>
+      <c r="I117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>204.9710859665115</v>
+      </c>
+      <c r="C118" t="n">
+        <v>243.8251434270446</v>
+      </c>
+      <c r="D118" t="n">
+        <v>217.923265895175</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>2</v>
+      </c>
+      <c r="G118" t="n">
+        <v>212.1150871372558</v>
+      </c>
+      <c r="H118" t="n">
+        <v>2</v>
+      </c>
+      <c r="I118" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>